<commit_message>
incorporate last changes from review
</commit_message>
<xml_diff>
--- a/resources/terminology.xlsx
+++ b/resources/terminology.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/jdurazo_worldbank_org/Documents/COUNTRIES/QA-GB/DataQA-GB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{4B91808B-50F0-274E-8222-8FC3931BB77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{740FD5FE-700A-4B15-B13C-94D180E6EFA8}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{4B91808B-50F0-274E-8222-8FC3931BB77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21CD712-BAF4-4B50-863D-EA1D1F47274F}"/>
   <bookViews>
     <workbookView xWindow="2508" yWindow="2640" windowWidth="17592" windowHeight="8376" xr2:uid="{5F610E7D-516F-4D0E-9C99-25E102E12365}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Concept</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A survey is the process of collecting, aggregating, and analyzing the responses from those questionnaires. </t>
   </si>
 </sst>
 </file>
@@ -481,14 +484,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCDB658-A979-4647-B5F9-26FDB723BC77}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" customWidth="1"/>
+    <col min="2" max="2" width="99" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -591,6 +594,9 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>